<commit_message>
protocol bug: sort by
</commit_message>
<xml_diff>
--- a/Experiments/221220_serine_titrate/biosyn_pl.xlsx
+++ b/Experiments/221220_serine_titrate/biosyn_pl.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryancardiff/Documents/Carothers/ARPA-E/Experiments/221220_serine_titrate/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryancardiff/Documents/GitHub/WHISPR/Experiments/221220_serine_titrate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72697755-D81B-EB49-A30E-158E55E1B206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A6A3EC-2F5E-4C4D-94FE-03010E0B105C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="1240" windowWidth="27640" windowHeight="16140" xr2:uid="{C3B1D29E-B544-3246-8B60-4AE0CA7FC900}"/>
   </bookViews>
@@ -461,7 +461,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>